<commit_message>
compara respuestas sin orden
</commit_message>
<xml_diff>
--- a/comparacion_resultados.xlsx
+++ b/comparacion_resultados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,11 +441,6 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Respuesta</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
           <t>Estado</t>
         </is>
       </c>
@@ -458,11 +453,6 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
           <t>Correcto</t>
         </is>
       </c>
@@ -475,11 +465,6 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
           <t>Correcto</t>
         </is>
       </c>
@@ -492,12 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Incorrecto</t>
+          <t>Correcto</t>
         </is>
       </c>
     </row>
@@ -509,11 +489,6 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
           <t>Correcto</t>
         </is>
       </c>
@@ -526,11 +501,6 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
           <t>Correcto</t>
         </is>
       </c>
@@ -543,11 +513,6 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
           <t>Correcto</t>
         </is>
       </c>
@@ -560,11 +525,6 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
           <t>Correcto</t>
         </is>
       </c>
@@ -577,11 +537,6 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
           <t>Correcto</t>
         </is>
       </c>
@@ -594,11 +549,6 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
           <t>Correcto</t>
         </is>
       </c>
@@ -611,11 +561,6 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
           <t>Correcto</t>
         </is>
       </c>
@@ -628,11 +573,6 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
           <t>Correcto</t>
         </is>
       </c>
@@ -645,11 +585,6 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
           <t>Correcto</t>
         </is>
       </c>
@@ -662,11 +597,6 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
           <t>Correcto</t>
         </is>
       </c>
@@ -679,11 +609,6 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
           <t>Correcto</t>
         </is>
       </c>
@@ -696,11 +621,6 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
           <t>Correcto</t>
         </is>
       </c>
@@ -713,11 +633,6 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
           <t>Correcto</t>
         </is>
       </c>
@@ -730,11 +645,6 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
           <t>Correcto</t>
         </is>
       </c>
@@ -747,11 +657,6 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
           <t>Correcto</t>
         </is>
       </c>
@@ -764,11 +669,6 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
           <t>Correcto</t>
         </is>
       </c>
@@ -780,11 +680,6 @@
         </is>
       </c>
       <c r="B21" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
         <is>
           <t>Correcto</t>
         </is>

</xml_diff>